<commit_message>
update the input of decision tree
</commit_message>
<xml_diff>
--- a/EuclideanDistance.xlsx
+++ b/EuclideanDistance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxb/Desktop/Practice/001_hkbu_2_final_exam/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxb/Desktop/Practice/001_hkbu_2_final_exam/7930_BDA_exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126A782E-8EB6-A24F-BB00-7523F8E886D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F77480A-DEA7-1948-A066-8EF9913BA061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29600" windowHeight="19200" xr2:uid="{55DB38B1-E4A7-46EC-8B7A-8D5782EED99B}"/>
   </bookViews>
@@ -1957,16 +1957,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>467894</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>189163</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>239294</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>74863</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>287421</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>24732</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>84221</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100932</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2293,8 +2293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E17D757-4C73-4CA4-9ECF-DF2B53F429AE}">
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
some tiny adust about ipynb & excel  file
</commit_message>
<xml_diff>
--- a/EuclideanDistance.xlsx
+++ b/EuclideanDistance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxb/Desktop/Practice/001_hkbu_2_final_exam/7930_BDA_exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F77480A-DEA7-1948-A066-8EF9913BA061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A887CCB3-1E47-8F47-9524-94CCCAF42D8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29600" windowHeight="19200" xr2:uid="{55DB38B1-E4A7-46EC-8B7A-8D5782EED99B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,12 +63,20 @@
     <t>C4_dist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>SSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +92,17 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +121,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -119,7 +148,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -127,6 +156,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2293,8 +2331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E17D757-4C73-4CA4-9ECF-DF2B53F429AE}">
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2552,11 +2590,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
-      <c r="B19">
+    <row r="19" spans="1:8">
+      <c r="B19" s="3">
         <v>5</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>10</v>
       </c>
       <c r="E19">
@@ -2572,11 +2610,11 @@
         <v>4.7487914681699035</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
-      <c r="B20">
+    <row r="20" spans="1:8">
+      <c r="B20" s="3">
         <v>5</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>5</v>
       </c>
       <c r="E20">
@@ -2592,11 +2630,11 @@
         <v>1.3552618543578767</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
-      <c r="B21">
+    <row r="21" spans="1:8">
+      <c r="B21" s="3">
         <v>5</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>8</v>
       </c>
       <c r="E21">
@@ -2612,11 +2650,11 @@
         <v>2.8749445424997293</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
-      <c r="B22">
+    <row r="22" spans="1:8">
+      <c r="B22" s="3">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>5</v>
       </c>
       <c r="E22">
@@ -2632,11 +2670,11 @@
         <v>2.747912008810192</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
-      <c r="B23">
+    <row r="23" spans="1:8">
+      <c r="B23" s="3">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>4</v>
       </c>
       <c r="E23">
@@ -2652,11 +2690,11 @@
         <v>3.0672729362262698</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
-      <c r="B24">
+    <row r="24" spans="1:8">
+      <c r="B24" s="3">
         <v>1</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>2</v>
       </c>
       <c r="E24">
@@ -2672,11 +2710,11 @@
         <v>4.3729222471468479</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
-      <c r="B25">
+    <row r="25" spans="1:8">
+      <c r="B25" s="3">
         <v>8</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>4</v>
       </c>
       <c r="E25">
@@ -2692,16 +2730,22 @@
         <v>4.5175395145262565</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
-      <c r="B27">
+    <row r="27" spans="1:8">
+      <c r="A27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4">
         <f>AVERAGE(B19:B25)</f>
         <v>3.7142857142857144</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <f>AVERAGE(C19:C25)</f>
         <v>5.4285714285714288</v>
       </c>
-      <c r="H27">
+      <c r="G27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="4">
         <f>SUM(H19:H25)</f>
         <v>23.684644571737074</v>
       </c>

</xml_diff>